<commit_message>
license update, readme, and manufacturing files
</commit_message>
<xml_diff>
--- a/iris-128b/pcb/iris-128b/manufacturing/bom/iris128b-bom.xlsx
+++ b/iris-128b/pcb/iris-128b/manufacturing/bom/iris128b-bom.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="Z:\[00] Project Folders\Emma_All_Projects\Emma_128ch_Headstage\pcb\pcb design\iris-128b\manufacturing\bom\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Emmak\Documents\GitHub\iris-128\iris-128b\pcb\iris-128b\manufacturing\bom\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E4015327-FB14-465F-B7EE-21EA722D9962}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{56B062D6-661C-4F0F-AF48-18BF6B856CCA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="19090" yWindow="-110" windowWidth="25820" windowHeight="13900" xr2:uid="{4F0840F9-FDF6-4062-89F4-E22A5CC7C0F6}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{4F0840F9-FDF6-4062-89F4-E22A5CC7C0F6}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -145,9 +145,6 @@
     <t>SMD</t>
   </si>
   <si>
-    <t>C2, C3, C24, C5, C1, C25, C8, C10, C22, C17, C16, C23, C4, C20, C13, C6, C11, C26, C19, C14, C21, C15, C7, C12</t>
-  </si>
-  <si>
     <t/>
   </si>
   <si>
@@ -163,9 +160,6 @@
     <t>QFN</t>
   </si>
   <si>
-    <t>R2, R3, R4, R5</t>
-  </si>
-  <si>
     <t>RC0201FR-07100RL</t>
   </si>
   <si>
@@ -175,9 +169,6 @@
     <t>Digikey『 』311-100MTR-ND</t>
   </si>
   <si>
-    <t>R7, LVDS1, LVDS3, LVDS2, LVDS4, LVDS5, LVDS8, LVDS7, LVDS6, R10, R9, R11, R8</t>
-  </si>
-  <si>
     <t>RMCF0201ZT0R00</t>
   </si>
   <si>
@@ -187,9 +178,6 @@
     <t>Digikey『 』RMCF0201ZT0R00TR-ND</t>
   </si>
   <si>
-    <t>C9, C28, C18, C27, C31, C32, C30, C29</t>
-  </si>
-  <si>
     <t>TMK063B7103KP-F</t>
   </si>
   <si>
@@ -215,6 +203,18 @@
   </si>
   <si>
     <t>Intan</t>
+  </si>
+  <si>
+    <t>C1-C24</t>
+  </si>
+  <si>
+    <t>R10, R11, R2, R3, R4, R5, R6, R7, R8, R9</t>
+  </si>
+  <si>
+    <t>LVDS1, LVDS3, LVDS2, LVDS4, LVDS5, LVDS8, LVDS7, LVDS6, R1</t>
+  </si>
+  <si>
+    <t>C25-32</t>
   </si>
 </sst>
 </file>
@@ -635,12 +635,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DC684751-6EF0-4B28-8DA3-2F56178B9ED8}">
   <dimension ref="A1:H8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G4" sqref="G4"/>
+    <sheetView tabSelected="1" zoomScale="87" workbookViewId="0">
+      <selection activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
+    <col min="2" max="2" width="99.08984375" customWidth="1"/>
     <col min="3" max="3" width="12" customWidth="1"/>
     <col min="4" max="4" width="29.26953125" customWidth="1"/>
     <col min="5" max="5" width="29.1796875" customWidth="1"/>
@@ -675,7 +676,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:8" ht="87.5" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:8" ht="25" x14ac:dyDescent="0.35">
       <c r="A2" s="1">
         <v>1</v>
       </c>
@@ -701,24 +702,24 @@
         <v>12</v>
       </c>
     </row>
-    <row r="3" spans="1:8" ht="50" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A3" s="1">
         <v>2</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>13</v>
+        <v>33</v>
       </c>
       <c r="C3" s="1">
         <v>24</v>
       </c>
       <c r="D3" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E3" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="E3" s="2" t="s">
+      <c r="F3" s="1" t="s">
         <v>15</v>
-      </c>
-      <c r="F3" s="1" t="s">
-        <v>16</v>
       </c>
       <c r="G3" s="1" t="s">
         <v>12</v>
@@ -732,46 +733,46 @@
         <v>3</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C4" s="1">
         <v>8</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="G4" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="H4" s="2" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="5" spans="1:8" ht="50" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A5" s="1">
         <v>4</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>19</v>
+        <v>34</v>
       </c>
       <c r="C5" s="1">
         <v>4</v>
       </c>
       <c r="D5" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="E5" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="F5" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="E5" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="F5" s="1" t="s">
-        <v>22</v>
-      </c>
       <c r="G5" s="1" t="s">
         <v>12</v>
       </c>
@@ -779,24 +780,24 @@
         <v>12</v>
       </c>
     </row>
-    <row r="6" spans="1:8" ht="62.5" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:8" ht="25" x14ac:dyDescent="0.35">
       <c r="A6" s="1">
         <v>5</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>23</v>
+        <v>35</v>
       </c>
       <c r="C6" s="1">
         <v>13</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="F6" s="1" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="G6" s="1" t="s">
         <v>12</v>
@@ -805,24 +806,24 @@
         <v>12</v>
       </c>
     </row>
-    <row r="7" spans="1:8" ht="187.5" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:8" ht="50" x14ac:dyDescent="0.35">
       <c r="A7" s="1">
         <v>6</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>27</v>
+        <v>36</v>
       </c>
       <c r="C7" s="1">
         <v>8</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="E7" s="2" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="F7" s="1" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="G7" s="1" t="s">
         <v>12</v>
@@ -831,24 +832,24 @@
         <v>12</v>
       </c>
     </row>
-    <row r="8" spans="1:8" ht="62.5" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:8" ht="25" x14ac:dyDescent="0.35">
       <c r="A8" s="1">
         <v>7</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="C8" s="1">
         <v>1</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="E8" s="2" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="F8" s="1" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="G8" s="1" t="s">
         <v>12</v>

</xml_diff>